<commit_message>
Updated the IMC protocol to introduce an option of a manual pause and a 4C overnight incubation. Merged the CODEX_single_stain and CODEX_multicycle protocols into one protocol and added the options for FFPE and Antibody_Screening modes in the *MODIFIABLE RUN PARAMETER* section. Setting Antibody_Screening to False makes this protocol run like CODEX_multicycle, setting it to true makes it run like CODEX_single_stain
</commit_message>
<xml_diff>
--- a/protocols/IMC/labware layout.xlsx
+++ b/protocols/IMC/labware layout.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dana\PycharmProjects\ot2-scripts\protocols\IMC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CD00AAF-B136-4A4B-9113-6F93E14B10BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21D0AA8D-CE71-479B-B15B-51851082D72C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="30960" windowHeight="16920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="48">
   <si>
     <t xml:space="preserve">Antibody plate (96-well plate, sealed with a pierceable sealing sheet, i.e. aluminum foil) </t>
   </si>
@@ -143,6 +143,39 @@
   </si>
   <si>
     <t>RuO4</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>Blocking Mix 1</t>
+  </si>
+  <si>
+    <t>Blocking Mix 2</t>
+  </si>
+  <si>
+    <t>Blocking Mix 3</t>
+  </si>
+  <si>
+    <t>Blocking Mix 4</t>
+  </si>
+  <si>
+    <t>Blocking Mix 5</t>
+  </si>
+  <si>
+    <t>Blocking Mix 6</t>
+  </si>
+  <si>
+    <t>Blocking Mix 7</t>
+  </si>
+  <si>
+    <t>Blocking Mix 8</t>
+  </si>
+  <si>
+    <t>Blocking Mix 9</t>
+  </si>
+  <si>
+    <t>3% BSA in Maxpar PBS</t>
   </si>
 </sst>
 </file>
@@ -291,7 +324,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -305,7 +338,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -314,19 +346,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -346,6 +365,19 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -568,7 +600,7 @@
   <dimension ref="A1:T1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O17" sqref="O17"/>
+      <selection activeCell="O8" sqref="O8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -648,76 +680,78 @@
       <c r="A4" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="F4" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="G4" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="H4" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="I4" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="J4" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="K4" s="8"/>
-      <c r="L4" s="8"/>
-      <c r="M4" s="8"/>
-      <c r="N4" s="20" t="s">
+      <c r="B4" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="H4" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="I4" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="J4" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="K4" s="7"/>
+      <c r="L4" s="7"/>
+      <c r="M4" s="7"/>
+      <c r="N4" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="O4" s="7"/>
+      <c r="O4" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="5" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="21" t="s">
-        <v>27</v>
-      </c>
-      <c r="C5" s="21" t="s">
-        <v>28</v>
-      </c>
-      <c r="D5" s="21" t="s">
-        <v>29</v>
-      </c>
-      <c r="E5" s="21" t="s">
-        <v>30</v>
-      </c>
-      <c r="F5" s="21" t="s">
-        <v>31</v>
-      </c>
-      <c r="G5" s="21" t="s">
-        <v>32</v>
-      </c>
-      <c r="H5" s="21" t="s">
-        <v>33</v>
-      </c>
-      <c r="I5" s="21" t="s">
-        <v>34</v>
-      </c>
-      <c r="J5" s="21" t="s">
-        <v>35</v>
-      </c>
-      <c r="K5" s="8"/>
-      <c r="L5" s="8"/>
-      <c r="M5" s="8"/>
-      <c r="N5" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="H5" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="I5" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="J5" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="K5" s="7"/>
+      <c r="L5" s="7"/>
+      <c r="M5" s="7"/>
+      <c r="N5" s="12" t="s">
         <v>26</v>
       </c>
       <c r="O5" s="4"/>
@@ -726,37 +760,37 @@
       <c r="A6" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="22" t="s">
-        <v>36</v>
-      </c>
-      <c r="C6" s="22" t="s">
-        <v>36</v>
-      </c>
-      <c r="D6" s="22" t="s">
-        <v>36</v>
-      </c>
-      <c r="E6" s="22" t="s">
-        <v>36</v>
-      </c>
-      <c r="F6" s="22" t="s">
-        <v>36</v>
-      </c>
-      <c r="G6" s="22" t="s">
-        <v>36</v>
-      </c>
-      <c r="H6" s="22" t="s">
-        <v>36</v>
-      </c>
-      <c r="I6" s="22" t="s">
-        <v>36</v>
-      </c>
-      <c r="J6" s="22" t="s">
-        <v>36</v>
-      </c>
-      <c r="K6" s="6"/>
-      <c r="L6" s="6"/>
-      <c r="M6" s="6"/>
-      <c r="N6" s="20" t="s">
+      <c r="B6" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="E6" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="F6" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="G6" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="H6" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="I6" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="J6" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="K6" s="7"/>
+      <c r="L6" s="7"/>
+      <c r="M6" s="7"/>
+      <c r="N6" s="12" t="s">
         <v>26</v>
       </c>
       <c r="O6" s="4"/>
@@ -765,131 +799,151 @@
       <c r="A7" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="6"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6"/>
-      <c r="H7" s="6"/>
-      <c r="I7" s="6"/>
-      <c r="J7" s="6"/>
+      <c r="B7" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="C7" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="D7" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="E7" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="F7" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="G7" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="H7" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="I7" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="J7" s="14" t="s">
+        <v>36</v>
+      </c>
       <c r="K7" s="6"/>
       <c r="L7" s="6"/>
       <c r="M7" s="6"/>
-      <c r="N7" s="4"/>
-      <c r="O7" s="23"/>
-      <c r="P7" s="24"/>
-      <c r="Q7" s="24"/>
-      <c r="R7" s="24"/>
-      <c r="S7" s="24"/>
-      <c r="T7" s="24"/>
+      <c r="N7" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="O7" s="15"/>
+      <c r="P7" s="16"/>
+      <c r="Q7" s="16"/>
+      <c r="R7" s="16"/>
+      <c r="S7" s="16"/>
+      <c r="T7" s="16"/>
     </row>
     <row r="8" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
         <v>16</v>
       </c>
       <c r="B8" s="6"/>
-      <c r="C8" s="9"/>
+      <c r="C8" s="8"/>
       <c r="D8" s="6"/>
-      <c r="E8" s="9"/>
+      <c r="E8" s="8"/>
       <c r="F8" s="6"/>
-      <c r="G8" s="9"/>
-      <c r="H8" s="9"/>
-      <c r="I8" s="9"/>
-      <c r="J8" s="9"/>
-      <c r="K8" s="9"/>
-      <c r="L8" s="9"/>
-      <c r="M8" s="9"/>
-      <c r="N8" s="10"/>
-      <c r="O8" s="24"/>
-      <c r="P8" s="24"/>
-      <c r="Q8" s="24"/>
-      <c r="R8" s="24"/>
-      <c r="S8" s="24"/>
-      <c r="T8" s="24"/>
+      <c r="G8" s="8"/>
+      <c r="H8" s="8"/>
+      <c r="I8" s="8"/>
+      <c r="J8" s="8"/>
+      <c r="K8" s="8"/>
+      <c r="L8" s="8"/>
+      <c r="M8" s="8"/>
+      <c r="N8" s="9"/>
+      <c r="O8" s="16"/>
+      <c r="P8" s="16"/>
+      <c r="Q8" s="16"/>
+      <c r="R8" s="16"/>
+      <c r="S8" s="16"/>
+      <c r="T8" s="16"/>
     </row>
     <row r="9" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
         <v>17</v>
       </c>
       <c r="B9" s="6"/>
-      <c r="C9" s="9"/>
+      <c r="C9" s="8"/>
       <c r="D9" s="6"/>
-      <c r="E9" s="9"/>
+      <c r="E9" s="8"/>
       <c r="F9" s="6"/>
-      <c r="G9" s="9"/>
-      <c r="H9" s="9"/>
-      <c r="I9" s="9"/>
-      <c r="J9" s="9"/>
-      <c r="K9" s="9"/>
-      <c r="L9" s="9"/>
-      <c r="M9" s="9"/>
-      <c r="N9" s="10"/>
-      <c r="O9" s="24"/>
-      <c r="P9" s="24"/>
-      <c r="Q9" s="24"/>
-      <c r="R9" s="24"/>
-      <c r="S9" s="24"/>
-      <c r="T9" s="24"/>
+      <c r="G9" s="8"/>
+      <c r="H9" s="8"/>
+      <c r="I9" s="8"/>
+      <c r="J9" s="8"/>
+      <c r="K9" s="8"/>
+      <c r="L9" s="8"/>
+      <c r="M9" s="8"/>
+      <c r="N9" s="9"/>
+      <c r="O9" s="16"/>
+      <c r="P9" s="16"/>
+      <c r="Q9" s="16"/>
+      <c r="R9" s="16"/>
+      <c r="S9" s="16"/>
+      <c r="T9" s="16"/>
     </row>
     <row r="10" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
         <v>18</v>
       </c>
       <c r="B10" s="6"/>
-      <c r="C10" s="9"/>
+      <c r="C10" s="8"/>
       <c r="D10" s="6"/>
-      <c r="E10" s="9"/>
+      <c r="E10" s="8"/>
       <c r="F10" s="6"/>
-      <c r="G10" s="9"/>
-      <c r="H10" s="9"/>
-      <c r="I10" s="9"/>
-      <c r="J10" s="9"/>
-      <c r="K10" s="9"/>
-      <c r="L10" s="9"/>
-      <c r="M10" s="9"/>
-      <c r="N10" s="10"/>
-      <c r="O10" s="24"/>
-      <c r="P10" s="25"/>
-      <c r="Q10" s="25"/>
-      <c r="R10" s="25"/>
-      <c r="S10" s="25"/>
-      <c r="T10" s="24"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="8"/>
+      <c r="I10" s="8"/>
+      <c r="J10" s="8"/>
+      <c r="K10" s="8"/>
+      <c r="L10" s="8"/>
+      <c r="M10" s="8"/>
+      <c r="N10" s="9"/>
+      <c r="O10" s="16"/>
+      <c r="P10" s="17"/>
+      <c r="Q10" s="17"/>
+      <c r="R10" s="17"/>
+      <c r="S10" s="17"/>
+      <c r="T10" s="16"/>
     </row>
     <row r="11" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
         <v>19</v>
       </c>
       <c r="B11" s="6"/>
-      <c r="C11" s="9"/>
+      <c r="C11" s="8"/>
       <c r="D11" s="6"/>
-      <c r="E11" s="9"/>
+      <c r="E11" s="8"/>
       <c r="F11" s="6"/>
-      <c r="G11" s="9"/>
-      <c r="H11" s="9"/>
-      <c r="I11" s="9"/>
-      <c r="J11" s="9"/>
-      <c r="K11" s="9"/>
-      <c r="L11" s="9"/>
-      <c r="M11" s="9"/>
-      <c r="N11" s="10"/>
-      <c r="O11" s="24"/>
-      <c r="P11" s="26"/>
-      <c r="Q11" s="27"/>
-      <c r="R11" s="25"/>
-      <c r="S11" s="25"/>
-      <c r="T11" s="24"/>
+      <c r="G11" s="8"/>
+      <c r="H11" s="8"/>
+      <c r="I11" s="8"/>
+      <c r="J11" s="8"/>
+      <c r="K11" s="8"/>
+      <c r="L11" s="8"/>
+      <c r="M11" s="8"/>
+      <c r="N11" s="9"/>
+      <c r="O11" s="16"/>
+      <c r="P11" s="18"/>
+      <c r="Q11" s="19"/>
+      <c r="R11" s="17"/>
+      <c r="S11" s="17"/>
+      <c r="T11" s="16"/>
     </row>
     <row r="12" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="1"/>
-      <c r="N12" s="10"/>
-      <c r="O12" s="24"/>
-      <c r="P12" s="26"/>
-      <c r="Q12" s="27"/>
-      <c r="R12" s="25"/>
-      <c r="S12" s="25"/>
-      <c r="T12" s="24"/>
+      <c r="N12" s="9"/>
+      <c r="O12" s="16"/>
+      <c r="P12" s="18"/>
+      <c r="Q12" s="19"/>
+      <c r="R12" s="17"/>
+      <c r="S12" s="17"/>
+      <c r="T12" s="16"/>
     </row>
     <row r="13" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="4" t="s">
@@ -898,13 +952,13 @@
       <c r="H13" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="N13" s="10"/>
-      <c r="O13" s="24"/>
-      <c r="P13" s="28"/>
-      <c r="Q13" s="26"/>
-      <c r="R13" s="27"/>
-      <c r="S13" s="25"/>
-      <c r="T13" s="24"/>
+      <c r="N13" s="9"/>
+      <c r="O13" s="16"/>
+      <c r="P13" s="20"/>
+      <c r="Q13" s="18"/>
+      <c r="R13" s="19"/>
+      <c r="S13" s="17"/>
+      <c r="T13" s="16"/>
     </row>
     <row r="14" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B14" s="4">
@@ -943,231 +997,231 @@
       <c r="M14" s="1">
         <v>12</v>
       </c>
-      <c r="N14" s="12" t="s">
+      <c r="N14" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="O14" s="24"/>
-      <c r="P14" s="28"/>
-      <c r="Q14" s="26"/>
-      <c r="R14" s="27"/>
-      <c r="S14" s="25"/>
-      <c r="T14" s="24"/>
+      <c r="O14" s="16"/>
+      <c r="P14" s="20"/>
+      <c r="Q14" s="18"/>
+      <c r="R14" s="19"/>
+      <c r="S14" s="17"/>
+      <c r="T14" s="16"/>
     </row>
     <row r="15" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="16" t="s">
+      <c r="A15" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="B15" s="19" t="s">
+      <c r="B15" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="C15" s="19" t="s">
+      <c r="C15" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="D15" s="19" t="s">
+      <c r="D15" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="E15" s="19"/>
-      <c r="F15" s="18"/>
-      <c r="G15" s="18"/>
-      <c r="H15" s="18"/>
-      <c r="I15" s="18"/>
-      <c r="J15" s="18"/>
-      <c r="K15" s="13"/>
-      <c r="L15" s="13"/>
-      <c r="M15" s="13"/>
-      <c r="N15" s="10" t="s">
+      <c r="E15" s="26"/>
+      <c r="F15" s="27"/>
+      <c r="G15" s="27"/>
+      <c r="H15" s="27"/>
+      <c r="I15" s="27"/>
+      <c r="J15" s="27"/>
+      <c r="K15" s="21"/>
+      <c r="L15" s="21"/>
+      <c r="M15" s="21"/>
+      <c r="N15" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="O15" s="24"/>
-      <c r="P15" s="28"/>
-      <c r="Q15" s="26"/>
-      <c r="R15" s="27"/>
-      <c r="S15" s="25"/>
-      <c r="T15" s="24"/>
+      <c r="O15" s="16"/>
+      <c r="P15" s="20"/>
+      <c r="Q15" s="18"/>
+      <c r="R15" s="19"/>
+      <c r="S15" s="17"/>
+      <c r="T15" s="16"/>
     </row>
     <row r="16" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="17"/>
-      <c r="B16" s="14"/>
-      <c r="C16" s="14"/>
-      <c r="D16" s="14"/>
-      <c r="E16" s="14"/>
-      <c r="F16" s="14"/>
-      <c r="G16" s="14"/>
-      <c r="H16" s="14"/>
-      <c r="I16" s="14"/>
-      <c r="J16" s="14"/>
-      <c r="K16" s="14"/>
-      <c r="L16" s="14"/>
-      <c r="M16" s="14"/>
-      <c r="O16" s="24"/>
-      <c r="P16" s="28"/>
-      <c r="Q16" s="26"/>
-      <c r="R16" s="27"/>
-      <c r="S16" s="25"/>
-      <c r="T16" s="24"/>
+      <c r="A16" s="25"/>
+      <c r="B16" s="22"/>
+      <c r="C16" s="22"/>
+      <c r="D16" s="22"/>
+      <c r="E16" s="22"/>
+      <c r="F16" s="22"/>
+      <c r="G16" s="22"/>
+      <c r="H16" s="22"/>
+      <c r="I16" s="22"/>
+      <c r="J16" s="22"/>
+      <c r="K16" s="22"/>
+      <c r="L16" s="22"/>
+      <c r="M16" s="22"/>
+      <c r="O16" s="16"/>
+      <c r="P16" s="20"/>
+      <c r="Q16" s="18"/>
+      <c r="R16" s="19"/>
+      <c r="S16" s="17"/>
+      <c r="T16" s="16"/>
     </row>
     <row r="17" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="17"/>
-      <c r="B17" s="14"/>
-      <c r="C17" s="14"/>
-      <c r="D17" s="14"/>
-      <c r="E17" s="14"/>
-      <c r="F17" s="14"/>
-      <c r="G17" s="14"/>
-      <c r="H17" s="14"/>
-      <c r="I17" s="14"/>
-      <c r="J17" s="14"/>
-      <c r="K17" s="14"/>
-      <c r="L17" s="14"/>
-      <c r="M17" s="14"/>
-      <c r="N17" s="10"/>
-      <c r="O17" s="24"/>
-      <c r="P17" s="28"/>
-      <c r="Q17" s="26"/>
-      <c r="R17" s="27"/>
-      <c r="S17" s="25"/>
-      <c r="T17" s="24"/>
+      <c r="A17" s="25"/>
+      <c r="B17" s="22"/>
+      <c r="C17" s="22"/>
+      <c r="D17" s="22"/>
+      <c r="E17" s="22"/>
+      <c r="F17" s="22"/>
+      <c r="G17" s="22"/>
+      <c r="H17" s="22"/>
+      <c r="I17" s="22"/>
+      <c r="J17" s="22"/>
+      <c r="K17" s="22"/>
+      <c r="L17" s="22"/>
+      <c r="M17" s="22"/>
+      <c r="N17" s="9"/>
+      <c r="O17" s="16"/>
+      <c r="P17" s="20"/>
+      <c r="Q17" s="18"/>
+      <c r="R17" s="19"/>
+      <c r="S17" s="17"/>
+      <c r="T17" s="16"/>
     </row>
     <row r="18" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="17"/>
-      <c r="B18" s="14"/>
-      <c r="C18" s="14"/>
-      <c r="D18" s="14"/>
-      <c r="E18" s="14"/>
-      <c r="F18" s="14"/>
-      <c r="G18" s="14"/>
-      <c r="H18" s="14"/>
-      <c r="I18" s="14"/>
-      <c r="J18" s="14"/>
-      <c r="K18" s="14"/>
-      <c r="L18" s="14"/>
-      <c r="M18" s="14"/>
-      <c r="N18" s="10"/>
-      <c r="O18" s="24"/>
-      <c r="P18" s="28"/>
-      <c r="Q18" s="26"/>
-      <c r="R18" s="27"/>
-      <c r="S18" s="25"/>
-      <c r="T18" s="24"/>
+      <c r="A18" s="25"/>
+      <c r="B18" s="22"/>
+      <c r="C18" s="22"/>
+      <c r="D18" s="22"/>
+      <c r="E18" s="22"/>
+      <c r="F18" s="22"/>
+      <c r="G18" s="22"/>
+      <c r="H18" s="22"/>
+      <c r="I18" s="22"/>
+      <c r="J18" s="22"/>
+      <c r="K18" s="22"/>
+      <c r="L18" s="22"/>
+      <c r="M18" s="22"/>
+      <c r="N18" s="9"/>
+      <c r="O18" s="16"/>
+      <c r="P18" s="20"/>
+      <c r="Q18" s="18"/>
+      <c r="R18" s="19"/>
+      <c r="S18" s="17"/>
+      <c r="T18" s="16"/>
     </row>
     <row r="19" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="17"/>
-      <c r="B19" s="14"/>
-      <c r="C19" s="14"/>
-      <c r="D19" s="14"/>
-      <c r="E19" s="14"/>
-      <c r="F19" s="14"/>
-      <c r="G19" s="14"/>
-      <c r="H19" s="14"/>
-      <c r="I19" s="14"/>
-      <c r="J19" s="14"/>
-      <c r="K19" s="14"/>
-      <c r="L19" s="14"/>
-      <c r="M19" s="14"/>
-      <c r="N19" s="10"/>
-      <c r="O19" s="24"/>
-      <c r="P19" s="28"/>
-      <c r="Q19" s="26"/>
-      <c r="R19" s="27"/>
-      <c r="S19" s="25"/>
-      <c r="T19" s="24"/>
+      <c r="A19" s="25"/>
+      <c r="B19" s="22"/>
+      <c r="C19" s="22"/>
+      <c r="D19" s="22"/>
+      <c r="E19" s="22"/>
+      <c r="F19" s="22"/>
+      <c r="G19" s="22"/>
+      <c r="H19" s="22"/>
+      <c r="I19" s="22"/>
+      <c r="J19" s="22"/>
+      <c r="K19" s="22"/>
+      <c r="L19" s="22"/>
+      <c r="M19" s="22"/>
+      <c r="N19" s="9"/>
+      <c r="O19" s="16"/>
+      <c r="P19" s="20"/>
+      <c r="Q19" s="18"/>
+      <c r="R19" s="19"/>
+      <c r="S19" s="17"/>
+      <c r="T19" s="16"/>
     </row>
     <row r="20" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="17"/>
-      <c r="B20" s="15"/>
-      <c r="C20" s="15"/>
-      <c r="D20" s="15"/>
-      <c r="E20" s="15"/>
-      <c r="F20" s="15"/>
-      <c r="G20" s="15"/>
-      <c r="H20" s="15"/>
-      <c r="I20" s="15"/>
-      <c r="J20" s="15"/>
-      <c r="K20" s="15"/>
-      <c r="L20" s="15"/>
-      <c r="M20" s="15"/>
-      <c r="N20" s="10"/>
-      <c r="O20" s="24"/>
-      <c r="P20" s="28"/>
-      <c r="Q20" s="26"/>
-      <c r="R20" s="27"/>
-      <c r="S20" s="25"/>
-      <c r="T20" s="24"/>
+      <c r="A20" s="25"/>
+      <c r="B20" s="23"/>
+      <c r="C20" s="23"/>
+      <c r="D20" s="23"/>
+      <c r="E20" s="23"/>
+      <c r="F20" s="23"/>
+      <c r="G20" s="23"/>
+      <c r="H20" s="23"/>
+      <c r="I20" s="23"/>
+      <c r="J20" s="23"/>
+      <c r="K20" s="23"/>
+      <c r="L20" s="23"/>
+      <c r="M20" s="23"/>
+      <c r="N20" s="9"/>
+      <c r="O20" s="16"/>
+      <c r="P20" s="20"/>
+      <c r="Q20" s="18"/>
+      <c r="R20" s="19"/>
+      <c r="S20" s="17"/>
+      <c r="T20" s="16"/>
     </row>
     <row r="21" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="O21" s="24"/>
-      <c r="P21" s="28"/>
-      <c r="Q21" s="26"/>
-      <c r="R21" s="27"/>
-      <c r="S21" s="25"/>
-      <c r="T21" s="24"/>
+      <c r="O21" s="16"/>
+      <c r="P21" s="20"/>
+      <c r="Q21" s="18"/>
+      <c r="R21" s="19"/>
+      <c r="S21" s="17"/>
+      <c r="T21" s="16"/>
     </row>
     <row r="22" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="O22" s="24"/>
-      <c r="P22" s="28"/>
-      <c r="Q22" s="25"/>
-      <c r="R22" s="25"/>
-      <c r="S22" s="25"/>
-      <c r="T22" s="24"/>
+      <c r="O22" s="16"/>
+      <c r="P22" s="20"/>
+      <c r="Q22" s="17"/>
+      <c r="R22" s="17"/>
+      <c r="S22" s="17"/>
+      <c r="T22" s="16"/>
     </row>
     <row r="23" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="O23" s="24"/>
-      <c r="P23" s="25"/>
-      <c r="Q23" s="25"/>
-      <c r="R23" s="25"/>
-      <c r="S23" s="25"/>
-      <c r="T23" s="24"/>
+      <c r="O23" s="16"/>
+      <c r="P23" s="17"/>
+      <c r="Q23" s="17"/>
+      <c r="R23" s="17"/>
+      <c r="S23" s="17"/>
+      <c r="T23" s="16"/>
     </row>
     <row r="24" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C24" s="11"/>
-      <c r="D24" s="11"/>
-      <c r="E24" s="11"/>
-      <c r="O24" s="24"/>
-      <c r="P24" s="25"/>
-      <c r="Q24" s="25"/>
-      <c r="R24" s="25"/>
-      <c r="S24" s="25"/>
-      <c r="T24" s="24"/>
+      <c r="C24" s="10"/>
+      <c r="D24" s="10"/>
+      <c r="E24" s="10"/>
+      <c r="O24" s="16"/>
+      <c r="P24" s="17"/>
+      <c r="Q24" s="17"/>
+      <c r="R24" s="17"/>
+      <c r="S24" s="17"/>
+      <c r="T24" s="16"/>
     </row>
     <row r="25" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C25" s="11"/>
-      <c r="D25" s="11"/>
-      <c r="E25" s="11"/>
+      <c r="C25" s="10"/>
+      <c r="D25" s="10"/>
+      <c r="E25" s="10"/>
     </row>
     <row r="26" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C26" s="11"/>
-      <c r="D26" s="11"/>
-      <c r="E26" s="11"/>
+      <c r="C26" s="10"/>
+      <c r="D26" s="10"/>
+      <c r="E26" s="10"/>
     </row>
     <row r="27" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C27" s="11"/>
-      <c r="D27" s="11"/>
-      <c r="E27" s="11"/>
+      <c r="C27" s="10"/>
+      <c r="D27" s="10"/>
+      <c r="E27" s="10"/>
     </row>
     <row r="28" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C28" s="11"/>
-      <c r="D28" s="11"/>
-      <c r="E28" s="11"/>
+      <c r="C28" s="10"/>
+      <c r="D28" s="10"/>
+      <c r="E28" s="10"/>
     </row>
     <row r="29" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C29" s="11"/>
-      <c r="D29" s="11"/>
-      <c r="E29" s="11"/>
+      <c r="C29" s="10"/>
+      <c r="D29" s="10"/>
+      <c r="E29" s="10"/>
     </row>
     <row r="30" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C30" s="11"/>
-      <c r="D30" s="11"/>
-      <c r="E30" s="11"/>
+      <c r="C30" s="10"/>
+      <c r="D30" s="10"/>
+      <c r="E30" s="10"/>
     </row>
     <row r="31" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C31" s="11"/>
-      <c r="D31" s="11"/>
-      <c r="E31" s="11"/>
+      <c r="C31" s="10"/>
+      <c r="D31" s="10"/>
+      <c r="E31" s="10"/>
     </row>
     <row r="32" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C32" s="11"/>
-      <c r="D32" s="11"/>
-      <c r="E32" s="11"/>
+      <c r="C32" s="10"/>
+      <c r="D32" s="10"/>
+      <c r="E32" s="10"/>
     </row>
     <row r="33" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="34" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>